<commit_message>
data preparing tranformers creation
</commit_message>
<xml_diff>
--- a/data/erp/test_anomaly.xlsx
+++ b/data/erp/test_anomaly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\watex\data\erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA0874B-CDDD-4155-9BDF-9303D86A2219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B022F29-D5B5-45F3-B3EF-FE8289AE7971}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="6375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>pk</t>
   </si>
@@ -32,18 +32,6 @@
   </si>
   <si>
     <t>Rho</t>
-  </si>
-  <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>CB2P</t>
   </si>
 </sst>
 </file>
@@ -744,7 +732,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>93</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>93</c:v>
@@ -753,7 +741,7 @@
                   <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>93</c:v>
@@ -765,7 +753,7 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>130</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>163</c:v>
@@ -1545,16 +1533,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1879,15 +1867,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,14 +1888,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1918,19 +1900,11 @@
         <v>1093010</v>
       </c>
       <c r="D2" s="1">
-        <v>93</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1944,7 +1918,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -1958,7 +1932,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -1969,10 +1943,10 @@
         <v>1093033</v>
       </c>
       <c r="D5">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>40</v>
       </c>
@@ -1988,7 +1962,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -2002,7 +1976,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60</v>
       </c>
@@ -2016,7 +1990,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70</v>
       </c>
@@ -2027,10 +2001,10 @@
         <v>1093063</v>
       </c>
       <c r="D9">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -2043,11 +2017,9 @@
       <c r="D10" s="1">
         <v>163</v>
       </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
+      <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90</v>
       </c>
@@ -2061,7 +2033,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -2075,7 +2047,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>110</v>
       </c>
@@ -2089,7 +2061,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
@@ -2103,7 +2075,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>130</v>
       </c>
@@ -2117,7 +2089,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>140</v>
       </c>

</xml_diff>